<commit_message>
Started on SQLscripts: usertables finished
</commit_message>
<xml_diff>
--- a/design/database/databaserelaties.xlsx
+++ b/design/database/databaserelaties.xlsx
@@ -214,7 +214,7 @@
     <t>RegistrationDate::DateTime</t>
   </si>
   <si>
-    <t>Preferred Language::DateTime</t>
+    <t>Preferred Language::String</t>
   </si>
   <si>
     <t>Password::String</t>
@@ -252,6 +252,7 @@
   <fonts count="7">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -272,18 +273,21 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <color rgb="00800000"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <color rgb="00FF0000"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <color rgb="00000000"/>
       <sz val="10"/>
@@ -376,33 +380,33 @@
   </sheetPr>
   <dimension ref="A2:T34"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="U5" activeCellId="0" pane="topLeft" sqref="U5"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A19" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G35" activeCellId="0" pane="topLeft" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6352941176471"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3803921568627"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.7725490196078"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.2901960784314"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.4039215686275"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.356862745098"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.4274509803922"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.0745098039216"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.643137254902"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="31.321568627451"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="15.5372549019608"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="17.356862745098"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.2823529411765"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7254901960784"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.4588235294118"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8627450980392"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.0392156862745"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.4196078431373"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.4823529411765"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.4470588235294"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.4980392156863"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.1647058823529"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.7607843137255"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="31.4745098039216"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="15.6117647058824"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="17.4470588235294"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.3529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="F2" s="0" t="s">
         <v>0</v>
       </c>
@@ -410,7 +414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="3">
       <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
@@ -444,7 +448,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="23.85" outlineLevel="0" r="4">
       <c r="L4" s="0" t="s">
         <v>12</v>
       </c>
@@ -464,7 +468,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="5">
       <c r="E5" s="0" t="s">
         <v>15</v>
       </c>
@@ -475,7 +479,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="6">
       <c r="E6" s="7" t="s">
         <v>18</v>
       </c>
@@ -498,7 +502,7 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="23.85" outlineLevel="0" r="7">
       <c r="E7" s="0" t="s">
         <v>24</v>
       </c>
@@ -524,7 +528,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="8">
       <c r="M8" s="7" t="s">
         <v>27</v>
       </c>
@@ -538,7 +542,7 @@
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="23.85" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
         <v>30</v>
       </c>
@@ -558,7 +562,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="8" t="s">
         <v>5</v>
       </c>
@@ -568,7 +572,7 @@
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>12</v>
       </c>
@@ -576,12 +580,12 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="G12" s="0" t="s">
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>33</v>
       </c>
@@ -607,7 +611,7 @@
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="23.85" outlineLevel="0" r="14">
       <c r="A14" s="7" t="s">
         <v>40</v>
       </c>
@@ -639,7 +643,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="23.85" outlineLevel="0" r="15">
       <c r="A15" s="6" t="s">
         <v>25</v>
       </c>
@@ -659,7 +663,7 @@
         <v>46</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="16">
       <c r="F16" s="1" t="s">
         <v>5</v>
       </c>
@@ -676,7 +680,7 @@
         <v>49</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="F17" s="0" t="s">
         <v>12</v>
       </c>
@@ -687,7 +691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="19">
       <c r="B19" s="0" t="s">
         <v>50</v>
       </c>
@@ -695,7 +699,7 @@
         <v>51</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="20">
       <c r="B20" s="8" t="s">
         <v>2</v>
       </c>
@@ -721,7 +725,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="B21" s="0" t="s">
         <v>12</v>
       </c>
@@ -750,7 +754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="35.05" outlineLevel="0" r="22">
       <c r="F22" s="0" t="s">
         <v>12</v>
       </c>
@@ -767,12 +771,12 @@
         <v>57</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="B24" s="0" t="s">
         <v>58</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="B25" s="8" t="s">
         <v>2</v>
       </c>
@@ -783,17 +787,17 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="B26" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="B28" s="0" t="s">
         <v>59</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="29">
       <c r="B29" s="1" t="s">
         <v>5</v>
       </c>
@@ -840,7 +844,7 @@
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="35.05" outlineLevel="0" r="30">
       <c r="B30" s="0" t="s">
         <v>12</v>
       </c>
@@ -884,17 +888,17 @@
         <v>57</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="32">
       <c r="B32" s="0" t="s">
         <v>72</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="B33" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="B34" s="0" t="s">
         <v>12</v>
       </c>

</xml_diff>